<commit_message>
Update binary file in infomax_functions_templates with new data
</commit_message>
<xml_diff>
--- a/infomax_functions_templetes/인포맥스함수_항섭/함수 예시 List.xlsx
+++ b/infomax_functions_templetes/인포맥스함수_항섭/함수 예시 List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr codeName="현재_통합_문서"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepositories\infomax_supabase_bot\infomax_functions_templetes\인포맥스함수_항섭\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FB0DAE-76F1-488E-91C3-5C40B2675E56}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F8CB5D-D7DF-4B52-8E52-EE7865F08FA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
   <si>
     <t>현재가</t>
   </si>
@@ -87,6 +87,147 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>IRS KRW (Qr VS Qr 91D CD91) 06개월</t>
+  </si>
+  <si>
+    <t>IRS KRW (Qr VS Qr 91D CD91) 09개월</t>
+  </si>
+  <si>
+    <t>IRS KRW (Qr VS Qr 91D CD91) 01년</t>
+  </si>
+  <si>
+    <t>IRS KRW (Qr VS Qr 91D CD91) 18개월</t>
+  </si>
+  <si>
+    <t>IRS KRW (Qr VS Qr 91D CD91) 02년</t>
+  </si>
+  <si>
+    <t>IRS KRW (Qr VS Qr 91D CD91) 03년</t>
+  </si>
+  <si>
+    <t>IRS KRW (Qr VS Qr 91D CD91) 04년</t>
+  </si>
+  <si>
+    <t>IRS KRW (Qr VS Qr 91D CD91) 25년</t>
+  </si>
+  <si>
+    <t>IRS KRW (Qr VS Qr 91D CD91) 30년</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>IRSTP1KRW06M</t>
+  </si>
+  <si>
+    <t>IRSTP1KRW09M</t>
+  </si>
+  <si>
+    <t>IRSTP1KRW01Y</t>
+  </si>
+  <si>
+    <t>IRSTP1KRW18M</t>
+  </si>
+  <si>
+    <t>IRSTP1KRW02Y</t>
+  </si>
+  <si>
+    <t>IRSTP1KRW03Y</t>
+  </si>
+  <si>
+    <t>IRSTP1KRW04Y</t>
+  </si>
+  <si>
+    <t>IRSTP1KRW25Y</t>
+  </si>
+  <si>
+    <t>IRSTP1KRW30Y</t>
+  </si>
+  <si>
+    <t>매수시가</t>
+  </si>
+  <si>
+    <t>매수고가</t>
+  </si>
+  <si>
+    <t>매수저가</t>
+  </si>
+  <si>
+    <t>매수종가</t>
+  </si>
+  <si>
+    <t>매수전일대비</t>
+  </si>
+  <si>
+    <t>매도시가</t>
+  </si>
+  <si>
+    <t>매도고가</t>
+  </si>
+  <si>
+    <t>매도저가</t>
+  </si>
+  <si>
+    <t>매도종가</t>
+  </si>
+  <si>
+    <t>매도전일대비</t>
+  </si>
+  <si>
+    <t>MID시가</t>
+  </si>
+  <si>
+    <t>MID고가</t>
+  </si>
+  <si>
+    <t>MID저가</t>
+  </si>
+  <si>
+    <t>MID종가</t>
+  </si>
+  <si>
+    <t>MID전일대비</t>
+  </si>
+  <si>
+    <t>스프레드</t>
+  </si>
+  <si>
+    <t>RATE_ID</t>
+  </si>
+  <si>
+    <t>MMKT_FIELD_ID</t>
+  </si>
+  <si>
+    <t>DATA_TYPE</t>
+  </si>
+  <si>
+    <t>DATA_ID</t>
+  </si>
+  <si>
+    <t>FIELD_ID</t>
+  </si>
+  <si>
+    <t>CNHUSD3F3L6M</t>
+  </si>
+  <si>
+    <t>MID</t>
+  </si>
+  <si>
+    <t>CRST25USDCNH06M</t>
+  </si>
+  <si>
+    <t>IMDH(Market, Code, Field, StartDay, EndDay, Count, Option)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMDP(Market, Code, Field, Date, Option)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMDT(SchName, Code, Field, Count, SchDate, SchVal1, SchVal2, Option)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -152,13 +293,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -193,7 +335,7 @@
         <tr r="F18" s="1"/>
       </tp>
       <tp>
-        <v>152300</v>
+        <v>151600</v>
         <stp/>
         <stp>P</stp>
         <stp>0</stp>
@@ -215,6 +357,78 @@
         <stp>20260106</stp>
         <stp/>
         <tr r="F15" s="1"/>
+      </tp>
+      <tp>
+        <v>2.5000000000000001E-2</v>
+        <stp/>
+        <stp>P</stp>
+        <stp>0</stp>
+        <stp>IR</stp>
+        <stp>IRSTP1KRW01Y</stp>
+        <stp>매도전일대비</stp>
+        <stp>20260106</stp>
+        <stp/>
+        <tr r="O30" s="1"/>
+      </tp>
+      <tp>
+        <v>0.03</v>
+        <stp/>
+        <stp>P</stp>
+        <stp>0</stp>
+        <stp>IR</stp>
+        <stp>IRSTP1KRW01Y</stp>
+        <stp>스프레드</stp>
+        <stp>20260106</stp>
+        <stp/>
+        <tr r="U30" s="1"/>
+      </tp>
+      <tp>
+        <v>2.7250000000000001</v>
+        <stp/>
+        <stp>P</stp>
+        <stp>0</stp>
+        <stp>IR</stp>
+        <stp>IRSTP1KRW01Y</stp>
+        <stp>MID시가</stp>
+        <stp>20260106</stp>
+        <stp/>
+        <tr r="P30" s="1"/>
+      </tp>
+      <tp>
+        <v>2.75</v>
+        <stp/>
+        <stp>P</stp>
+        <stp>0</stp>
+        <stp>IR</stp>
+        <stp>IRSTP1KRW01Y</stp>
+        <stp>MID종가</stp>
+        <stp>20260106</stp>
+        <stp/>
+        <tr r="S30" s="1"/>
+      </tp>
+      <tp>
+        <v>2.7225000000000001</v>
+        <stp/>
+        <stp>P</stp>
+        <stp>0</stp>
+        <stp>IR</stp>
+        <stp>IRSTP1KRW01Y</stp>
+        <stp>MID저가</stp>
+        <stp>20260106</stp>
+        <stp/>
+        <tr r="R30" s="1"/>
+      </tp>
+      <tp>
+        <v>2.75</v>
+        <stp/>
+        <stp>P</stp>
+        <stp>0</stp>
+        <stp>IR</stp>
+        <stp>IRSTP1KRW01Y</stp>
+        <stp>MID고가</stp>
+        <stp>20260106</stp>
+        <stp/>
+        <tr r="Q30" s="1"/>
       </tp>
       <tp>
         <v>129300</v>
@@ -238,8 +452,8 @@
         <stp>현재가</stp>
         <stp>20260106</stp>
         <stp/>
+        <tr r="C7" s="1"/>
         <tr r="F14" s="1"/>
-        <tr r="C7" s="1"/>
       </tp>
       <tp>
         <v>141000</v>
@@ -276,6 +490,126 @@
         <stp>20260106</stp>
         <stp/>
         <tr r="F16" s="1"/>
+      </tp>
+      <tp>
+        <v>2.7650000000000001</v>
+        <stp/>
+        <stp>P</stp>
+        <stp>0</stp>
+        <stp>IR</stp>
+        <stp>IRSTP1KRW01Y</stp>
+        <stp>매도고가</stp>
+        <stp>20260106</stp>
+        <stp/>
+        <tr r="L30" s="1"/>
+      </tp>
+      <tp>
+        <v>2.74</v>
+        <stp/>
+        <stp>P</stp>
+        <stp>0</stp>
+        <stp>IR</stp>
+        <stp>IRSTP1KRW01Y</stp>
+        <stp>매도시가</stp>
+        <stp>20260106</stp>
+        <stp/>
+        <tr r="K30" s="1"/>
+      </tp>
+      <tp>
+        <v>2.7650000000000001</v>
+        <stp/>
+        <stp>P</stp>
+        <stp>0</stp>
+        <stp>IR</stp>
+        <stp>IRSTP1KRW01Y</stp>
+        <stp>매도종가</stp>
+        <stp>20260106</stp>
+        <stp/>
+        <tr r="N30" s="1"/>
+      </tp>
+      <tp>
+        <v>2.74</v>
+        <stp/>
+        <stp>P</stp>
+        <stp>0</stp>
+        <stp>IR</stp>
+        <stp>IRSTP1KRW01Y</stp>
+        <stp>매도저가</stp>
+        <stp>20260106</stp>
+        <stp/>
+        <tr r="M30" s="1"/>
+      </tp>
+      <tp>
+        <v>2.7349999999999999</v>
+        <stp/>
+        <stp>P</stp>
+        <stp>0</stp>
+        <stp>IR</stp>
+        <stp>IRSTP1KRW01Y</stp>
+        <stp>매수종가</stp>
+        <stp>20260106</stp>
+        <stp/>
+        <tr r="I30" s="1"/>
+      </tp>
+      <tp>
+        <v>2.7050000000000001</v>
+        <stp/>
+        <stp>P</stp>
+        <stp>0</stp>
+        <stp>IR</stp>
+        <stp>IRSTP1KRW01Y</stp>
+        <stp>매수저가</stp>
+        <stp>20260106</stp>
+        <stp/>
+        <tr r="H30" s="1"/>
+      </tp>
+      <tp>
+        <v>2.71</v>
+        <stp/>
+        <stp>P</stp>
+        <stp>0</stp>
+        <stp>IR</stp>
+        <stp>IRSTP1KRW01Y</stp>
+        <stp>매수시가</stp>
+        <stp>20260106</stp>
+        <stp/>
+        <tr r="F30" s="1"/>
+      </tp>
+      <tp>
+        <v>2.7349999999999999</v>
+        <stp/>
+        <stp>P</stp>
+        <stp>0</stp>
+        <stp>IR</stp>
+        <stp>IRSTP1KRW01Y</stp>
+        <stp>매수고가</stp>
+        <stp>20260106</stp>
+        <stp/>
+        <tr r="G30" s="1"/>
+      </tp>
+      <tp>
+        <v>2.5000000000000001E-2</v>
+        <stp/>
+        <stp>P</stp>
+        <stp>0</stp>
+        <stp>IR</stp>
+        <stp>IRSTP1KRW01Y</stp>
+        <stp>MID전일대비</stp>
+        <stp>20260106</stp>
+        <stp/>
+        <tr r="T30" s="1"/>
+      </tp>
+      <tp>
+        <v>2.5000000000000001E-2</v>
+        <stp/>
+        <stp>P</stp>
+        <stp>0</stp>
+        <stp>IR</stp>
+        <stp>IRSTP1KRW01Y</stp>
+        <stp>매수전일대비</stp>
+        <stp>20260106</stp>
+        <stp/>
+        <tr r="J30" s="1"/>
       </tp>
     </main>
   </volType>
@@ -546,17 +880,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B3:F18"/>
+  <dimension ref="B3:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="39.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="34.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
@@ -565,7 +901,7 @@
     <row r="4" spans="2:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C4" s="1">
         <f>_xll.IMDP("STK","N005930","현재가")</f>
-        <v>152300</v>
+        <v>151600</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -657,7 +993,7 @@
         <v>499.05</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
         <v>14</v>
       </c>
@@ -671,7 +1007,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C18" s="3" t="s">
         <v>17</v>
       </c>
@@ -684,6 +1020,290 @@
       <c r="F18">
         <f>_xll.IMDP("FX","USDSP_SMBCC","현재가","20260106")</f>
         <v>1445.5</v>
+      </c>
+    </row>
+    <row r="21" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C26" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O29" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="P29" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q29" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R29" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S29" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T29" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="U29" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="3:21" x14ac:dyDescent="0.3">
+      <c r="C30" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30">
+        <f>_xll.IMDP("IR","IRSTP1KRW01Y","매수시가","20260106")</f>
+        <v>2.71</v>
+      </c>
+      <c r="G30">
+        <f>_xll.IMDP("IR","IRSTP1KRW01Y","매수고가","20260106")</f>
+        <v>2.7349999999999999</v>
+      </c>
+      <c r="H30">
+        <f>_xll.IMDP("IR","IRSTP1KRW01Y","매수저가","20260106")</f>
+        <v>2.7050000000000001</v>
+      </c>
+      <c r="I30">
+        <f>_xll.IMDP("IR","IRSTP1KRW01Y","매수종가","20260106")</f>
+        <v>2.7349999999999999</v>
+      </c>
+      <c r="J30">
+        <f>_xll.IMDP("IR","IRSTP1KRW01Y","매수전일대비","20260106")</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K30">
+        <f>_xll.IMDP("IR","IRSTP1KRW01Y","매도시가","20260106")</f>
+        <v>2.74</v>
+      </c>
+      <c r="L30">
+        <f>_xll.IMDP("IR","IRSTP1KRW01Y","매도고가","20260106")</f>
+        <v>2.7650000000000001</v>
+      </c>
+      <c r="M30">
+        <f>_xll.IMDP("IR","IRSTP1KRW01Y","매도저가","20260106")</f>
+        <v>2.74</v>
+      </c>
+      <c r="N30">
+        <f>_xll.IMDP("IR","IRSTP1KRW01Y","매도종가","20260106")</f>
+        <v>2.7650000000000001</v>
+      </c>
+      <c r="O30">
+        <f>_xll.IMDP("IR","IRSTP1KRW01Y","매도전일대비","20260106")</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="P30">
+        <f>_xll.IMDP("IR","IRSTP1KRW01Y","MID시가","20260106")</f>
+        <v>2.7250000000000001</v>
+      </c>
+      <c r="Q30">
+        <f>_xll.IMDP("IR","IRSTP1KRW01Y","MID고가","20260106")</f>
+        <v>2.75</v>
+      </c>
+      <c r="R30">
+        <f>_xll.IMDP("IR","IRSTP1KRW01Y","MID저가","20260106")</f>
+        <v>2.7225000000000001</v>
+      </c>
+      <c r="S30">
+        <f>_xll.IMDP("IR","IRSTP1KRW01Y","MID종가","20260106")</f>
+        <v>2.75</v>
+      </c>
+      <c r="T30">
+        <f>_xll.IMDP("IR","IRSTP1KRW01Y","MID전일대비","20260106")</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="U30">
+        <f>_xll.IMDP("IR","IRSTP1KRW01Y","스프레드","20260106")</f>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" t="s">
+        <v>58</v>
+      </c>
+      <c r="G33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" t="s">
+        <v>62</v>
+      </c>
+      <c r="G34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new scripts for Infomax data extraction and testing, including environment checks, cleanup, and sample generation. Also, add new Excel files for data samples and templates.
</commit_message>
<xml_diff>
--- a/infomax_functions_templetes/인포맥스함수_항섭/함수 예시 List.xlsx
+++ b/infomax_functions_templetes/인포맥스함수_항섭/함수 예시 List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="현재_통합_문서"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepositories\infomax_supabase_bot\infomax_functions_templetes\인포맥스함수_항섭\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_repository\infomax_supabase_bot\infomax_functions_templetes\인포맥스함수_항섭\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F8CB5D-D7DF-4B52-8E52-EE7865F08FA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC9EAD6-0A4E-4BC6-8609-821CC42E40D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -335,7 +346,7 @@
         <tr r="F18" s="1"/>
       </tp>
       <tp>
-        <v>151600</v>
+        <v>151700</v>
         <stp/>
         <stp>P</stp>
         <stp>0</stp>
@@ -452,8 +463,8 @@
         <stp>현재가</stp>
         <stp>20260106</stp>
         <stp/>
+        <tr r="F14" s="1"/>
         <tr r="C7" s="1"/>
-        <tr r="F14" s="1"/>
       </tp>
       <tp>
         <v>141000</v>
@@ -882,8 +893,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B3:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -901,7 +912,7 @@
     <row r="4" spans="2:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C4" s="1">
         <f>_xll.IMDP("STK","N005930","현재가")</f>
-        <v>151600</v>
+        <v>151700</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>

</xml_diff>